<commit_message>
reporte usuarios y report resumen
</commit_message>
<xml_diff>
--- a/backend/resources/templates/reporte_cierre_actividades_final.xlsx
+++ b/backend/resources/templates/reporte_cierre_actividades_final.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>FECHA DE CIERRE</t>
   </si>
@@ -48,10 +48,10 @@
     <t>MES</t>
   </si>
   <si>
-    <t>REPORTE DE CIERRE DE REGISTRO DE METAS FÍSICAS DE ACTIVIDADES OPERATIVAS MES DE ENERO 2024</t>
-  </si>
-  <si>
     <t>N°</t>
+  </si>
+  <si>
+    <t>PERIODO</t>
   </si>
 </sst>
 </file>
@@ -124,10 +124,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,54 +408,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G4"/>
+  <dimension ref="A2:H4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="4"/>
+      <c r="H2" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="D2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -480,13 +483,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>

</xml_diff>